<commit_message>
클래스명 수정 urlEncode -> URLEncoder urlDecode -> URLDecoder
URLEncoder 패스에 한글이 포함된 경우 인코딩하도록 수정

타이틀 중복체크 선택적으로 수행하도록 수정 (※프로퍼티 읽어들이도록 수정 필요)
</commit_message>
<xml_diff>
--- a/scraper_Property.xlsx
+++ b/scraper_Property.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="25875" windowHeight="9855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t xml:space="preserve"> String id</t>
   </si>
@@ -226,6 +231,10 @@
   </si>
   <si>
     <t xml:space="preserve"> //img 와 같이 경로를 포함한 태그의 경우 경로를 외부에서 접근가능토록 절대경로로 재 가공한다.</t>
+  </si>
+  <si>
+    <t>Block</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -236,54 +245,94 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">제목&amp;lt/p&gt;과 같이 적을 경우, 태그가 남아있게 된다. 이런 내용까지도 제거하기 위함. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> //</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>타이틀 중복체크 수행여부</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">제목&amp;lt/p&gt;과 같이 적을 경우, 태그가 남아있게 된다. 이런 내용까지도 제거하기 위함. </t>
+      <t>.</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Block</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> boolean checkDuplicateTitle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="굴림"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -305,8 +354,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -317,15 +372,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -624,28 +681,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="50.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="139.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -661,7 +718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -669,7 +726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -677,7 +734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -685,7 +742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -693,7 +750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -701,7 +758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
@@ -709,7 +766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -717,7 +774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -725,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -733,7 +790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -741,7 +798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
@@ -749,7 +806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -757,7 +814,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
@@ -765,7 +822,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4">
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
@@ -773,7 +830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4">
       <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
@@ -781,7 +838,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4">
       <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
@@ -789,7 +846,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4">
       <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
@@ -797,7 +854,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4">
       <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
@@ -805,7 +862,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4">
       <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
@@ -813,7 +870,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4">
       <c r="B23" s="1" t="s">
         <v>41</v>
       </c>
@@ -821,7 +878,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4">
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -829,7 +886,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4">
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -837,7 +894,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4">
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
@@ -845,7 +902,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4">
       <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
@@ -853,7 +910,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4">
       <c r="B28" s="1" t="s">
         <v>51</v>
       </c>
@@ -861,15 +918,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4">
       <c r="B29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
       <c r="B30" s="1" t="s">
         <v>54</v>
       </c>
@@ -877,7 +934,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4">
       <c r="B31" s="1" t="s">
         <v>56</v>
       </c>
@@ -885,7 +942,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4">
       <c r="B32" s="1" t="s">
         <v>58</v>
       </c>
@@ -893,7 +950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4">
       <c r="B33" s="1" t="s">
         <v>60</v>
       </c>
@@ -901,7 +958,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4">
       <c r="B34" s="1" t="s">
         <v>62</v>
       </c>
@@ -909,7 +966,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4">
       <c r="B35" s="1" t="s">
         <v>64</v>
       </c>
@@ -917,7 +974,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4">
       <c r="B36" s="1" t="s">
         <v>66</v>
       </c>
@@ -925,12 +982,20 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4">
       <c r="B37" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D37" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -939,7 +1004,12 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -949,10 +1019,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -962,9 +1037,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>